<commit_message>
fixing some generate report logic
</commit_message>
<xml_diff>
--- a/client/src/comments.xlsx
+++ b/client/src/comments.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="560">
   <si>
     <t>EnglishName</t>
   </si>
@@ -178,7 +178,10 @@
     <t>Himantopus-mexicanus-H.-himantopus-melanurus-Himantopus-mexicanus-melanurus-H.-himantopus</t>
   </si>
   <si>
-    <t>Black-necked Stilt (Black-necked) [MG] - Himantopus mexicanus mexicanus</t>
+    <t>Black-necked Stilt (Black-necked)</t>
+  </si>
+  <si>
+    <t>Himantopus mexicanus mexicanus</t>
   </si>
   <si>
     <t>Black-necked Stilt [ssp.] - Himantopus mexicanus mexicanus</t>
@@ -187,7 +190,10 @@
     <t>Black-winged Stilt (Black-necked) [MG] - Himantopus himantopus mexicanus</t>
   </si>
   <si>
-    <t>Black-necked Stilt (White-backed) [MG] - Himantopus mexicanus melanurus</t>
+    <t>Black-necked Stilt (White-backed)</t>
+  </si>
+  <si>
+    <t>Himantopus mexicanus melanurus</t>
   </si>
   <si>
     <t>White-backed Stilt [MS] - Himantopus melanurus</t>
@@ -220,7 +226,10 @@
     <t>Anas flavirostris</t>
   </si>
   <si>
-    <t>Yellow-billed Teal (oxyptera) [MG] - Anas flavirostris oxyptera</t>
+    <t>Yellow-billed Teal (oxyptera)</t>
+  </si>
+  <si>
+    <t>Anas flavirostris oxyptera</t>
   </si>
   <si>
     <t>Yellow-billed Teal [ssp.] - Anas flavirostris oxyptera</t>
@@ -238,7 +247,7 @@
     <t>Penelope was the wife of the hero Odysseus in Greek mythology. She was the daughter of Icarius and Periboea.  Penelope had managed to keep all of her suitors at bay. She had told them she would choose a suitor once she finished weaving a burial shroud for her father-in-law, Laertes; however, every night, she would undo part of the shroud. Her plan was revealed by one of her servants, Melantho. Penelope eventually appeared in front of the suitors and said that she would marry the suitor that would be able to string Odysseus' bow and shoot an arrow through twelve axe heads. She already knew that this was a task that only her husband would have been able to achieve. None of the suitors was able to complete the task, and a disguised Odysseus asked to try; after being successful, he revealed himself and killed the suitors with the help of his son, the goddess Athena, and two of his herdsmen. Penelope, still not believing that this was her husband, told him to command the servant to move their bed. Odysseus protested saying that it was impossible as one of the legs of the bed was part of a living olive tree. Penelope finally accepted that this man was who he claimed to be, and the couple was reunited.</t>
   </si>
   <si>
-    <t>Penelope-hero-Odysseus-Penelope-Laertes;-Penelope-Odysseus'-Odysseus-Athena,-Penelope,-Odysseus-Penelope</t>
+    <t>Penelope*|hero*|Odysseus*|Penelope*|Laertes;*|Penelope*|Odysseus'*|Odysseus*|Athena,*|Penelope,*|Odysseus*|Penelope</t>
   </si>
   <si>
     <t>Spix's Guan</t>
@@ -271,7 +280,7 @@
     <t>Podiceps-rolland.</t>
   </si>
   <si>
-    <t>Rollandia:-rolland=</t>
+    <t>Rollandia:*|rolland=</t>
   </si>
   <si>
     <t>Rock Pigeon (Feral Pigeon)</t>
@@ -415,7 +424,7 @@
     <t>The two species of wedgebill - Geoffroy's Wedgebill and White-throated Wedgebill (Schistes albogularis) - formerly were classified as a single species, Wedge-billed Hummingbird (Schistes geoffroyi). The recurring mention of "wedge" in the English names for these hummingbirds refers to the tip of the bill, which is very narrow and sharply pointed; this unusual bill shape is quite distinctive, but is not readily seen in the field. Named for Etienne Geoffroy Saint-Hillaire (1772-1884) French zoologist.</t>
   </si>
   <si>
-    <t>(Schistes-albogularis)-(Schistes-geoffroyi).</t>
+    <t>(Schistes*|albogularis)*|(Schistes*|geoffroyi).</t>
   </si>
   <si>
     <t>Ssp. geoffroyi</t>
@@ -442,16 +451,19 @@
     <t xml:space="preserve">The Central and South American cyanotus subspecies group was formerly (e.g., Cory 1918, Chapman 1926) treated as a separate species from Mexican Colibri thalassinus, but they were treated as conspecific by Peters (1945).  Remsen et al. (2015) provided rationale for restoring species rank to the cyanotus group.  SACC proposal passed to treat cyanotus as a separate species and to restore the English name “Lesser Violetear.” </t>
   </si>
   <si>
-    <t>Lesser Violetear (Andean) [PG] - Colibri cyanotus cyanotus/crissalis</t>
+    <t>Ssp. crissalis</t>
+  </si>
+  <si>
+    <t>Lesser Violetear (Andean)</t>
+  </si>
+  <si>
+    <t>Colibri cyanotus cyanotus/crissalis</t>
   </si>
   <si>
     <t>Lesser Violetear [ssp.] - Colibri cyanotus crissalis</t>
   </si>
   <si>
     <t>Green Violet-ear (Mountain) [PG] - Colibri thalassinus [Mountain]</t>
-  </si>
-  <si>
-    <t>Ssp. crissalis</t>
   </si>
   <si>
     <r>
@@ -522,14 +534,19 @@
     <t>(Ocreatus addae)</t>
   </si>
   <si>
-    <t xml:space="preserve">The Racket tailed Puffleg was unknown in life but specimens existed in various London cabinets, whence a drawing was sent in 1832 by Mr. Underwood on behalf of Charles Stokes, a London stockbroker and collector. An article in Zootaxa 4200 (1): 083–108 2016 Biogeography and taxonomy of racket-tail hummingbirds (Aves: Trochilidae: Ocreatus): evidence for species delimitation from morphology and display behavior by KARL-L. SCHUCHMANN, ANDRÉ-A. WELLER &amp; DIETMAR JÜRGENS provided evidence from plumage and behavior that Ocreatus underwoodii should be treated as four species, with the subspecies addae, annae, and peruana elevated to species rank. If this is so the species would be thus: | White-booted Racket-tail O. underwoodii - Venezuela to W Ecuador | Peruvian Racket-tail O. peruvianus - E Ecuador to NE Peru | Anna’s Racket-tail O. annae - Pasco to Cuzco (endemic) | Rufous-booted Racket-tail O. addae - Bolivia (endemic)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocreatus-underwoodii-addae,-annae,-peruana  </t>
-  </si>
-  <si>
-    <t>Booted Racket-tail (Anna's) [EMG] - Ocreatus underwoodii annae</t>
+    <t>The Racket tailed Puffleg was unknown in life but specimens existed in various London cabinets, whence a drawing was sent in 1832 by Mr. Underwood on behalf of Charles Stokes, a London stockbroker and collector. An article in Zootaxa 4200 (1): 083–108 2016 Biogeography and taxonomy of racket-tail hummingbirds (Aves: Trochilidae: Ocreatus): evidence for species delimitation from morphology and display behavior by KARL-L. SCHUCHMANN, ANDRÉ-A. WELLER &amp; DIETMAR JÜRGENS provided evidence from plumage and behavior that Ocreatus underwoodii should be treated as four species, with the subspecies addae, annae, and peruana elevated to species rank. If this is so the species would be thus: | White-booted Racket-tail O. underwoodii - Venezuela to W Ecuador | Peruvian Racket-tail O. peruvianus - E Ecuador to NE Peru | Anna’s Racket-tail O. annae - Pasco to Cuzco (endemic) | Rufous-booted Racket-tail O. addae - Bolivia (endemic)</t>
+  </si>
+  <si>
+    <t>Ocreatus-underwoodii-addae,-annae,-peruana</t>
+  </si>
+  <si>
+    <t>White-booted*|Racket-tail*|O.*|underwoodii*|-*|Venezuela*|to*|W*|Ecuador*|Peruvian*|Racket-tail*|O.*|peruvianus*|-*|E*|Ecuador*|to*|NE*|Peru*|Anna’s*|Racket-tail*|O.*|annae*|-*|Pasco*|to*|Cuzco*|(endemic)*|Rufous-booted*|Racket-tail*|O.*|addae*|-*|Bolivia*|(endemic)</t>
+  </si>
+  <si>
+    <t>Booted Racket-tail (Anna's)</t>
+  </si>
+  <si>
+    <t>Ocreatus underwoodii annae</t>
   </si>
   <si>
     <t>Rufous-booted Racket-tail [ssp.] (E) - Ocreatus addae annae</t>
@@ -538,9 +555,6 @@
     <t>Booted Racket-tail (Rufous-booted) [PG] - Ocreatus underwoodii [Rufous-booted]</t>
   </si>
   <si>
-    <t>White-booted Racket-tail O. underwoodii - Venezuela to W Ecuador, Peruvian Racket-tail O. peruvianus - E Ecuador to NE Peru, Anna’s Racket-tail O. annae - Pasco to Cuzco (endemic), Rufous-booted Racket-tail O. addae - Bolivia (endemic).</t>
-  </si>
-  <si>
     <t>Gould's Jewelfront</t>
   </si>
   <si>
@@ -580,7 +594,7 @@
     <t>Eastern Mountaineer [MS] (E) - Oreonympha nobilis</t>
   </si>
   <si>
-    <t>Oreonympha:-nobilis:</t>
+    <t>Oreonympha:*|nobilis:</t>
   </si>
   <si>
     <t>Scaled Metaltail</t>
@@ -619,7 +633,13 @@
     <t>(Lophornis verreauxii)</t>
   </si>
   <si>
-    <t>Festive Coquette (Butterfly) [PG] - Lophornis chalybeus verreauxii/klagesi</t>
+    <t>Ssp. verreauxii</t>
+  </si>
+  <si>
+    <t>Festive Coquette (Butterfly)</t>
+  </si>
+  <si>
+    <t>Lophornis chalybeus verreauxii/klagesi</t>
   </si>
   <si>
     <t>Festive Coquette [ssp.] - Lophornis chalybeus verreauxii</t>
@@ -628,9 +648,6 @@
     <t>Butterfly Coquette [ssp.] - Lophornis verreauxii verreauxii</t>
   </si>
   <si>
-    <t>Ssp. verreauxii</t>
-  </si>
-  <si>
     <t>Sapphire-vented Puffleg</t>
   </si>
   <si>
@@ -649,7 +666,13 @@
     <t>(Eriocnemis sapphiropygia)</t>
   </si>
   <si>
-    <t>Sapphire-vented Puffleg (Coppery-naped) [EPG] - Eriocnemis luciani sapphiropygia/catharina</t>
+    <t>Ssp. sapphiropygia (E)</t>
+  </si>
+  <si>
+    <t>Sapphire-vented Puffleg (Coppery-naped)</t>
+  </si>
+  <si>
+    <t>Eriocnemis luciani sapphiropygia/catharina</t>
   </si>
   <si>
     <t>Sapphire-vented Puffleg [ssp.] - Eriocnemis luciani sapphiropygia</t>
@@ -658,9 +681,6 @@
     <t>Coppery-naped Puffleg [ssp.] - Eriocnemis sapphiropygia sapphiropygia</t>
   </si>
   <si>
-    <t>Ssp. sapphiropygia (E)</t>
-  </si>
-  <si>
     <t>White-tufted Sunbeam</t>
   </si>
   <si>
@@ -694,7 +714,13 @@
     <t>(Coeligena inca)</t>
   </si>
   <si>
-    <t>Collared Inca (Gould's) [PG] - Coeligena torquata inca/omissa</t>
+    <t>Ssp. omissa (E)</t>
+  </si>
+  <si>
+    <t>Collared Inca (Gould's)</t>
+  </si>
+  <si>
+    <t>Coeligena torquata inca/omissa</t>
   </si>
   <si>
     <t>Collared Inca [ssp.] - Coeligena torquata omissa</t>
@@ -703,9 +729,6 @@
     <t>Gould's Inca [ssp.] (RR) - Coeligena inca omissa</t>
   </si>
   <si>
-    <t>Ssp. omissa (E)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Violet-throated Starfrontlet </t>
   </si>
   <si>
@@ -724,7 +747,10 @@
     <t>(Coeligena osculans)</t>
   </si>
   <si>
-    <t>Violet-throated Starfrontlet (Cuzco) [EMG] - Coeligena violifer osculans</t>
+    <t>Violet-throated Starfrontlet (Cuzco)</t>
+  </si>
+  <si>
+    <t>Coeligena violifer osculans</t>
   </si>
   <si>
     <t>Violet-throated Starfrontlet [ssp.] (E) - Coeligena violifer osculans</t>
@@ -733,9 +759,6 @@
     <t>Cuzco Starfrontlet [MS] (E) - Coeligena osculans</t>
   </si>
   <si>
-    <t>Ssp. osculans (E)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Giant Hummingbird </t>
   </si>
   <si>
@@ -781,7 +804,10 @@
     <t>The old Gray-necked Wood-Rail has been split two ways – Russet-napped Wood-Rail Aramides albiventris of Mexico and the Caribbean slope of Costa Rica and the one we saw of the Pacific slope of Costa Rica to Argentina.</t>
   </si>
   <si>
-    <t>Gray-cowled Wood-Rail (Gray-cowled) [MG] - Aramides cajaneus cajaneus</t>
+    <t>Gray-cowled Wood-Rail (Gray-cowled)</t>
+  </si>
+  <si>
+    <t>Aramides cajaneus cajaneus</t>
   </si>
   <si>
     <t>Grey-necked Wood Rail [ssp.] - Aramides cajaneus cajaneus</t>
@@ -841,16 +867,16 @@
     <t xml:space="preserve">ruficollis-"falklandica")  </t>
   </si>
   <si>
-    <t>Turkey Vulture (Tropical) [MG] - Cathartes aura ruficollis</t>
-  </si>
-  <si>
-    <t>Turkey Vulture [ssp.] - Cathartes aura ruficollis</t>
-  </si>
-  <si>
-    <t>Turkey Vulture (South Temperate) [MG] - Cathartes aura jota</t>
-  </si>
-  <si>
-    <t>Turkey Vulture [ssp.] - Cathartes aura jota</t>
+    <t>Turkey Vulture (Tropical)</t>
+  </si>
+  <si>
+    <t>Cathartes aura ruficollis</t>
+  </si>
+  <si>
+    <t>Turkey Vulture (South Temperate)</t>
+  </si>
+  <si>
+    <t>Cathartes aura jota</t>
   </si>
   <si>
     <t xml:space="preserve">Tawny-bellied Screech-Owl </t>
@@ -864,10 +890,13 @@
 SACC: Sibley &amp; Monroe (1990) and König et al. (1999) treated usta as a separate species from Megascops watsonii based on vocal differences, but this was not followed by Ridgely &amp; Greenfield (2001). SACC proposal to recognize usta as a separate species from M. watsonii was rejected because of inadequate geographic sampling and analysis.  Dantas et al. (2015) found that M. watsonii was paraphyletic with respect to M. sanctaecatarinae and that the subspecies usta itself is a paraphyletic taxon.</t>
   </si>
   <si>
-    <t>O.-flammulatus)-flammulatus)-Megascops.-Otus-Megascops.-Megascops-M.-albogularis,-M.-choliba,-M.- koepckeae,-Megascops-watsonii-M. sanctaecatarinae-usta</t>
-  </si>
-  <si>
-    <t>Tawny-bellied Screech-Owl (Austral) [MG] - Megascops watsonii usta</t>
+    <t>Otus-O.-flammulatus)-Otus-flammulatus)-Megascops.-Otus-Megascops.-Megascops-M.-albogularis,-M.-choliba,-M.- koepckeae,-usta-Megascops-watsonii-M.-watsonii-M. sanctaecatarinae-usta</t>
+  </si>
+  <si>
+    <t>Tawny-bellied Screech-Owl (Austral)</t>
+  </si>
+  <si>
+    <t>Megascops watsonii usta</t>
   </si>
   <si>
     <t>Tawny-bellied Screech-Owl [ssp.] - Megascops watsonii usta</t>
@@ -890,7 +919,7 @@
     <t>From the Greek Pharo = Mantle or Cloak. Machrus = long.</t>
   </si>
   <si>
-    <t>Pharo-Machrus</t>
+    <t>Pharo*|Machrus</t>
   </si>
   <si>
     <t xml:space="preserve">Amazonian Trogon </t>
@@ -962,7 +991,7 @@
     <t>Named for the Purus River that runs from eastern Peru into Brazil.</t>
   </si>
   <si>
-    <t xml:space="preserve">Western Striolated-Puffbird </t>
+    <t>Western Striolated-Puffbird</t>
   </si>
   <si>
     <t>Nystalus obamai</t>
@@ -983,9 +1012,6 @@
     <t>Named for the former President of the United States, Barack Obama.</t>
   </si>
   <si>
-    <t>Western Striolated-Puffbird [MS] - Nystalus obamai</t>
-  </si>
-  <si>
     <t>Western Striolated Puffbird [MS] - Nystalus obamai</t>
   </si>
   <si>
@@ -1031,10 +1057,19 @@
     <t>Eubucco: Gr. eu fine, beautiful; Mod. L. bucco barbet. richardsonii: tribute to the surgeon, zoologist, botanist, geologist and Scottish explorer. Sir John Richardson-(1787-1865).</t>
   </si>
   <si>
-    <t>eu,bucco</t>
-  </si>
-  <si>
-    <t>Lemon-throated Barbet (Flame-throated) [PG] - Eubucco richardsoni aurantiicollis/purusianus</t>
+    <t>eu-bucco</t>
+  </si>
+  <si>
+    <t>Eubucco:*|richardsonii:</t>
+  </si>
+  <si>
+    <t>Ssp. aurantiicollis</t>
+  </si>
+  <si>
+    <t>Lemon-throated Barbet (Flame-throated)</t>
+  </si>
+  <si>
+    <t>Eubucco richardsoni aurantiicollis/purusianus</t>
   </si>
   <si>
     <t>Lemon-throated Barbet [ssp.] - Eubucco richardsoni aurantiicollis</t>
@@ -1043,12 +1078,6 @@
     <t>Flame-throated Barbet [ssp.] - Eubucco aurantiicollis aurantiicollis</t>
   </si>
   <si>
-    <t>Eubucco:-richardsonii:</t>
-  </si>
-  <si>
-    <t>Ssp. aurantiicollis</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chestnut-eared Aracari </t>
   </si>
   <si>
@@ -1070,7 +1099,10 @@
     <t>Black-throated Toucanet | (Aulacorhynchus atrogularis)</t>
   </si>
   <si>
-    <t>Southern Emerald-Toucanet (Black-throated) [PG] - Aulacorhynchus albivitta atrogularis/dimidiatus</t>
+    <t>Southern Emerald-Toucanet (Black-throated)</t>
+  </si>
+  <si>
+    <t>Aulacorhynchus albivitta atrogularis/dimidiatus</t>
   </si>
   <si>
     <t>Black-throated Toucanet - Aulacorhynchus atrogularis</t>
@@ -1274,16 +1306,19 @@
     <t>nanus-dubius-Pyrocephalus-rubinus-obscurus, Pyrocephalus-rubinus-Pyrocephalus.</t>
   </si>
   <si>
-    <t>Vermilion Flycatcher (Austral) [MG] - Pyrocephalus rubinus rubinus</t>
+    <t>Austral migrant.</t>
+  </si>
+  <si>
+    <t>Vermilion Flycatcher (Austral)</t>
+  </si>
+  <si>
+    <t>Pyrocephalus rubinus rubinus</t>
   </si>
   <si>
     <t>Scarlet Flycatcher [MS] - Pyrocephalus rubinus</t>
   </si>
   <si>
     <t>Common Vermilion Flycatcher (Austral) [MG] - Pyrocephalus rubinus rubinus</t>
-  </si>
-  <si>
-    <t>Austral migrant.</t>
   </si>
   <si>
     <t xml:space="preserve">Slaty-backed Chat-Tyrant </t>
@@ -1324,7 +1359,13 @@
     <t>SACC: García-Moreno et al. (1998) suggested that the plumage and genetic differences between subspecies groups north and south of the Marañon should be recognized at the species level, with Ochthoeca thoracica the name for the southern species. Ridgely &amp; Tudor (1994) reported that there are also vocal differences that would support this split. Ridgely &amp; Greenfield (2001) and Hilty (2003) further recognized Venezuelan nigrita as a separate species from O. cinnamomeiventris, as done by Cory &amp; Hellmayr (1927); see Zimmer (1937b) for the rationale for treating them all as conspecific based on plumage pattern, the treatment followed by Fitzpatrick (2004). SACC proposal needed.</t>
   </si>
   <si>
-    <t>Slaty-backed Chat-Tyrant (Maroon-belted) [PG] - Ochthoeca cinnamomeiventris thoracica/angustifasciata</t>
+    <t>Ssp. thoracica</t>
+  </si>
+  <si>
+    <t>Slaty-backed Chat-Tyrant (Maroon-belted)</t>
+  </si>
+  <si>
+    <t>Ochthoeca cinnamomeiventris thoracica/angustifasciata</t>
   </si>
   <si>
     <t>Maroon-belted Chat-Tyrant [ssp.] - Ochthoeca thoracica thoracica</t>
@@ -1333,9 +1374,6 @@
     <t>Chestnut-belted Chat-tyrant [ssp.] - Ochthoeca thoracica thoracica</t>
   </si>
   <si>
-    <t>Ssp. thoracica</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lemon-browed Flycatcher </t>
   </si>
   <si>
@@ -1364,6 +1402,9 @@
   </si>
   <si>
     <t>Tyrannus melancholicus</t>
+  </si>
+  <si>
+    <t>A widespread and common Neotropical kingbird, found in open lowlands from Mexico through Central America and most of South America. A very vocal species whose bright, ringing trills are often the first clue to its presence. Usually perches prominently in tree tops or on wires, from which it sallies in pursuit of flying insects. The identification of this species is usually straightforward when aided by voice, but also focus on the notched shape and olive-brown color of the tail, and the size of the bill. Sexes alike. – John van Dort</t>
   </si>
   <si>
     <t xml:space="preserve">Dwarf Tyrant-Manakin </t>
@@ -1403,7 +1444,7 @@
     <t>stolzmanni: In honor of Jan Sztolcman (1854-1928) Polish zoologist, collector in tropical America 1875-1883.</t>
   </si>
   <si>
-    <t>jew-rit</t>
+    <t>"jew-rit"</t>
   </si>
   <si>
     <t xml:space="preserve">Yungas Manakin </t>
@@ -1451,7 +1492,13 @@
     <t>NB: Chivi Vireo is one of the most widespread and common passerines of South America. This species consists of a complex mosaic of resident and migratory populations, however. Not only is there seasonal overlap, in the austral winter, between some resident populations and wintering populations from southern South America, but during the boreal winter there also is overlap between the same resident Chivi Vireos and wintering Red-eyed Vireos (Vireo olivaceus) from North America! For many years Chivi and Red-eyed vireos were considered to be the same species; this is understandable, given that they are very similar in appearance, but phylogenetic analysis of DNA sequence data reveals that Chivi is more closely related to Black-whiskered Vireo (Vireo altiloquus) than it is to Red-eyed. The general biology of Chivi Vireo probably is very similar to that of Red-eyed Vireo but, despite its abundance, Chivi Vireo is much less well studied.</t>
   </si>
   <si>
-    <t>Chivi Vireo (migratory) [PG] - Vireo chivi chivi/diversus</t>
+    <t>Ssp. chivi</t>
+  </si>
+  <si>
+    <t>Chivi Vireo (migratory)</t>
+  </si>
+  <si>
+    <t>Vireo chivi chivi/diversus</t>
   </si>
   <si>
     <t>Chivi Vireo [ssp.] - Vireo chivi chivi</t>
@@ -1460,9 +1507,6 @@
     <t>Red-eyed Vireo (Chivi) [PG] - Vireo olivaceus [Chivi]</t>
   </si>
   <si>
-    <t>Ssp. chivi</t>
-  </si>
-  <si>
     <t xml:space="preserve">House Wren </t>
   </si>
   <si>
@@ -1472,7 +1516,10 @@
     <t>Many authors (e.g., Hellmayr 1934, Pinto 1944, Phelps &amp; Phelps 1950a) formerly treated Neotropical mainland populations as a separate species T. musculus; see also Brumfield and Capparella (1996); this treatment was followed by Brewer (2001) and Kroodsma &amp; Brewer (2005). &lt;incorp. Paynter 1957?&gt; The Falklands population, T. a. cobbi, might also be best treated as a species (Woods 1993), as was done by Brewer (2001), Mazar Barnett &amp; Pearman (2001), Jaramillo (2003), and Kroodsma &amp; Brewer (2005). SACC proposal to treat cobbi as separate species did not pass. Campagna et al. (2012) provided additional evidence that cobbi merits species rank. SACC proposal passed to treat cobbi as separate species.</t>
   </si>
   <si>
-    <t>House Wren (Southern) [PG] - Troglodytes aedon [musculus Group]</t>
+    <t>House Wren (Southern)</t>
+  </si>
+  <si>
+    <t>Troglodytes aedon [musculus Group]</t>
   </si>
   <si>
     <t>House Wren - Troglodytes aedon</t>
@@ -1523,7 +1570,10 @@
     <t>(Kleinothraupis auricularis)</t>
   </si>
   <si>
-    <t>Black-capped Hemispingus (White-browed) [EMG] - Kleinothraupis atropileus auricularis</t>
+    <t>Black-capped Hemispingus (White-browed)</t>
+  </si>
+  <si>
+    <t>Kleinothraupis atropileus auricularis</t>
   </si>
   <si>
     <t>White-browed Hemispingus [MS] (E) - Hemispingus auricularis</t>
@@ -1547,7 +1597,13 @@
     <t>episcopus – a reference to the episcopal blue plumage of this species.</t>
   </si>
   <si>
-    <t>Blue-gray Tanager (White-edged) [PG] - Thraupis episcopus [episcopus Group]</t>
+    <t>episcopus</t>
+  </si>
+  <si>
+    <t>Blue-gray Tanager (White-edged)</t>
+  </si>
+  <si>
+    <t>Thraupis episcopus [episcopus Group]</t>
   </si>
   <si>
     <t>Blue-grey Tanager [ssp.] - Thraupis episcopus urubambae</t>
@@ -1556,15 +1612,6 @@
     <t>Blue-grey Tanager (White-edged) [PG] - Thraupis episcopus [White-edged]</t>
   </si>
   <si>
-    <t>episcopus</t>
-  </si>
-  <si>
-    <t>Ssp. urubambae (E) |</t>
-  </si>
-  <si>
-    <t>Ssp. johntoddzimmeri (E)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Paradise Tanager </t>
   </si>
   <si>
@@ -1595,7 +1642,7 @@
     <t>Tangara: Tupí name, Tangara= dancer, one who turns and skips, originally used for the manakins, but subsequently (Marcgrave 1648) transferred to other bright finch-like birds. schrankii: In honor of Prof. Franz von Paula Schrank (1747-1835) German theologian, botanist, entomologist, collector.</t>
   </si>
   <si>
-    <t>Tangara:-schrankii:</t>
+    <t>Tangara:*|schrankii:</t>
   </si>
   <si>
     <t xml:space="preserve">Chestnut-breasted Mountain-Finch </t>
@@ -1640,7 +1687,10 @@
     <t>A very common bird of the Andes throughout Peru and South America.</t>
   </si>
   <si>
-    <t>Rufous-collared Sparrow (Rufous-collared) [PG] - Zonotrichia capensis [capensis Group]</t>
+    <t>Rufous-collared Sparrow (Rufous-collared)</t>
+  </si>
+  <si>
+    <t>Zonotrichia capensis [capensis Group]</t>
   </si>
   <si>
     <t xml:space="preserve">Black-faced Brushfinch </t>
@@ -1670,7 +1720,10 @@
     <t>SACC: Ridgely &amp; Greenfield (2001) treated the northern subspecies chlorophrys as a separate species from Myiothlypis chrysogaster based on differences in descriptions of songs; see Zimmer (1949) for rationale for considering them sister taxa. SACC proposal to split chlorophrys from chrysogaster did not pass due to insufficient published data.</t>
   </si>
   <si>
-    <t>Golden-bellied Warbler (Golden-bellied) [EMG] - Myiothlypis chrysogaster chrysogaster</t>
+    <t>Golden-bellied Warbler (Golden-bellied)</t>
+  </si>
+  <si>
+    <t>Myiothlypis chrysogaster chrysogaster</t>
   </si>
   <si>
     <t>Cuzco Warbler [MS] (E) - Myiothlypis chrysogaster</t>
@@ -1714,7 +1767,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
       <sz val="12.0"/>
@@ -1756,7 +1808,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -1822,6 +1875,18 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <i/>
+      <sz val="12.0"/>
+      <color rgb="FF0070C0"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12.0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
       <b/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1849,20 +1914,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <i/>
-      <sz val="12.0"/>
-      <color rgb="FF366091"/>
-      <name val="Docs-Calibri"/>
-    </font>
-    <font>
       <b/>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FFCC00CC"/>
@@ -1897,18 +1952,19 @@
     <font>
       <sz val="12.0"/>
       <color rgb="FF555555"/>
-      <name val="Calibri"/>
+      <name val="Docs-Calibri"/>
     </font>
     <font>
       <sz val="12.0"/>
       <color rgb="FF555555"/>
-      <name val="Docs-Calibri"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12.0"/>
       <color rgb="FF0070C0"/>
       <name val="Docs-Calibri"/>
     </font>
+    <font/>
     <font>
       <sz val="12.0"/>
       <color rgb="FF800080"/>
@@ -1935,7 +1991,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1948,12 +2004,12 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1969,18 +2025,24 @@
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1996,140 +2058,149 @@
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="39" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="36" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="39" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="40" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="41" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -2420,7 +2491,7 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -2459,2049 +2530,2496 @@
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9" t="s">
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="8" t="s">
         <v>53</v>
       </c>
       <c r="Q7" s="1"/>
-      <c r="R7" s="2" t="s">
+      <c r="R7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="1"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="V7" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="W7" s="11" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="1" t="s">
+      <c r="W8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="Z7" s="12" t="s">
+      <c r="X8" s="10"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="AA7" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AB7" s="11"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="AA9" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4" t="s">
+      <c r="AB9" s="10"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="P9" s="9" t="s">
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="10"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S9" s="1"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="P11" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="R11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13" t="s">
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="V10" s="14" t="s">
+      <c r="B12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="W10" s="11" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="X10" s="11"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="P11" s="9" t="s">
+      <c r="W13" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="X13" s="10"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="P14" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="P12" s="1" t="s">
+      <c r="AC14" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
+    <row r="15">
+      <c r="A15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="P13" s="9" t="s">
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="P15" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
+    <row r="16">
+      <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="P14" s="1" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="P16" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="R14" s="2" t="s">
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S14" s="1"/>
-      <c r="T14" s="2"/>
-      <c r="AC14" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="P17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="R17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17" t="s">
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="AC17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="O15" s="18" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="O18" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="P16" s="9" t="s">
+      <c r="P18" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
+    <row r="19">
+      <c r="A19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="P17" s="9" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="P19" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
+    <row r="20">
+      <c r="A20" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="P18" s="9" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="P20" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="3" t="s">
+    <row r="21">
+      <c r="A21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="P19" s="9" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="P21" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="3" t="s">
+    <row r="22">
+      <c r="A22" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="P20" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="P22" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="3" t="s">
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="P21" s="9" t="s">
+      <c r="B23" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="19" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="P23" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B24" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="P22" s="20" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="P24" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="R22" s="1" t="s">
+    </row>
+    <row r="25">
+      <c r="A25" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
+      <c r="B25" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="P25" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="P23" s="9" t="s">
+      <c r="R25" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="19" t="s">
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="P24" s="21" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="P26" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="19" t="s">
+    <row r="27">
+      <c r="A27" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B27" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="P25" s="9" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="P27" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="R25" s="9" t="s">
+    </row>
+    <row r="28">
+      <c r="A28" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="S25" s="9"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="3" t="s">
+      <c r="B28" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="P28" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
+      <c r="R28" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="P26" s="9" t="s">
+      <c r="S28" s="8"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="AC26" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="3" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="P29" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="AC29" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I27" s="8" t="s">
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="O27" s="18" t="s">
+      <c r="B30" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="H30" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="AC27" s="2" t="s">
+      <c r="I30" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="AG27" s="22" t="s">
+      <c r="O30" s="19" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
+      <c r="P30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="AC30" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6" t="s">
+      <c r="AG30" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="I28" s="8" t="s">
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J28" s="23" t="s">
+      <c r="B31" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="L28" s="11" t="s">
+      <c r="F31" s="5"/>
+      <c r="G31" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="I31" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1" t="s">
+      <c r="J31" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="V28" s="14" t="s">
+      <c r="L31" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="W28" s="11" t="s">
+      <c r="P31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="X28" s="11"/>
-      <c r="AG28" s="22" t="s">
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="AG31" s="23" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
+    <row r="32">
+      <c r="A32" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B32" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="24"/>
+      <c r="L32" s="10"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="16" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="3" t="s">
+      <c r="W32" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="X32" s="10"/>
+      <c r="AG32" s="23"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
+      <c r="P33" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="3" t="s">
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="P31" s="24" t="s">
+      <c r="B34" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="R31" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S31" s="1"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="25" t="s">
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="s">
+      <c r="P35" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="R35" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P33" s="9" t="s">
+      <c r="S35" s="1"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="26" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="s">
+      <c r="B36" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="D36" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="B37" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I34" s="27" t="s">
+      <c r="P37" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="K34" s="28" t="s">
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="P34" s="9" t="s">
+      <c r="B38" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="R34" s="1" t="s">
+      <c r="H38" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="S34" s="1"/>
-      <c r="Y34" s="29" t="s">
+      <c r="I38" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="Z34" s="30" t="s">
+      <c r="K38" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="AA34" s="31" t="s">
+      <c r="P38" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="AB34" s="31"/>
-      <c r="AC34" s="1" t="s">
+      <c r="R38" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="3" t="s">
+      <c r="S38" s="1"/>
+      <c r="Y38" s="30"/>
+      <c r="Z38" s="31"/>
+      <c r="AA38" s="32"/>
+      <c r="AB38" s="32"/>
+      <c r="AC38" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B35" s="3" t="s">
+    </row>
+    <row r="39">
+      <c r="A39" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="P35" s="24" t="s">
+      <c r="B39" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="R35" s="1" t="s">
+      <c r="H39" s="27"/>
+      <c r="I39" s="28"/>
+      <c r="K39" s="29"/>
+      <c r="P39" s="8"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="V39" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="S35" s="1"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="25" t="s">
+      <c r="W39" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="32"/>
+      <c r="AB39" s="32"/>
+      <c r="AC39" s="1"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32" t="s">
+      <c r="B40" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="I36" s="27" t="s">
+      <c r="P40" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="O36" s="33" t="s">
+      <c r="R40" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="P36" s="9" t="s">
+      <c r="S40" s="1"/>
+    </row>
+    <row r="41" ht="1.5" customHeight="1">
+      <c r="A41" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="Q36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1" t="s">
+      <c r="B41" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="V36" s="14" t="s">
+      <c r="D41" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="W36" s="11" t="s">
+      <c r="I41" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="X36" s="11"/>
-      <c r="AC36" s="2" t="s">
+      <c r="O41" s="37" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
+      <c r="P41" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="Q41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="V41" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="W41" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="X41" s="10"/>
+      <c r="AC41" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Q37" s="1"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B38" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="Q42" s="1"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B43" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="B39" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C39" s="5" t="s">
+    <row r="44">
+      <c r="A44" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B44" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="I40" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="J40" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="L40" s="27" t="s">
+    <row r="45">
+      <c r="A45" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29" t="s">
+      <c r="B45" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="V40" s="36" t="s">
+      <c r="F45" s="5"/>
+      <c r="G45" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="W40" s="37" t="s">
+      <c r="I45" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="X40" s="37"/>
-      <c r="AG40" s="38" t="s">
+      <c r="J45" s="24" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="3" t="s">
+      <c r="L45" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="Q45" s="30"/>
+      <c r="R45" s="30"/>
+      <c r="S45" s="30"/>
+      <c r="T45" s="30"/>
+      <c r="U45" s="30"/>
+      <c r="V45" s="40"/>
+      <c r="W45" s="41"/>
+      <c r="X45" s="41"/>
+      <c r="AG45" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6" t="s">
+    </row>
+    <row r="46">
+      <c r="A46" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="B46" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="J41" s="23" t="s">
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="24"/>
+      <c r="L46" s="28"/>
+      <c r="Q46" s="30"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
+      <c r="U46" s="30"/>
+      <c r="V46" s="40" t="s">
         <v>207</v>
       </c>
-      <c r="L41" s="8" t="s">
+      <c r="W46" s="41" t="s">
         <v>208</v>
       </c>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="29"/>
-      <c r="S41" s="29"/>
-      <c r="T41" s="29"/>
-      <c r="U41" s="29" t="s">
+      <c r="X46" s="41"/>
+      <c r="AG46" s="42"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="V41" s="39" t="s">
+      <c r="B47" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="W41" s="37" t="s">
+      <c r="F47" s="5"/>
+      <c r="G47" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="X41" s="37"/>
-      <c r="AG41" s="18" t="s">
+      <c r="I47" s="7" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="3" t="s">
+      <c r="J47" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="L47" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="I42" s="11"/>
-      <c r="AD42" s="41" t="s">
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
+      <c r="U47" s="30"/>
+      <c r="V47" s="44"/>
+      <c r="W47" s="41"/>
+      <c r="X47" s="41"/>
+      <c r="AG47" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="AE42" s="11" t="s">
+    </row>
+    <row r="48">
+      <c r="A48" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="AG42" s="18" t="s">
+      <c r="B48" s="43" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="3" t="s">
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="24"/>
+      <c r="L48" s="7"/>
+      <c r="Q48" s="30"/>
+      <c r="R48" s="30"/>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
+      <c r="U48" s="30"/>
+      <c r="V48" s="44" t="s">
         <v>218</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="W48" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6" t="s">
+      <c r="X48" s="41"/>
+      <c r="AG48" s="19"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="I43" s="27" t="s">
+      <c r="B49" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="J43" s="6" t="s">
+      <c r="D49" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="I49" s="10"/>
+      <c r="AD49" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="L43" s="27" t="s">
+      <c r="AE49" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29" t="s">
+      <c r="AG49" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="V43" s="14" t="s">
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="W43" s="11" t="s">
+      <c r="B50" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="X43" s="11"/>
-      <c r="AG43" s="33" t="s">
+      <c r="F50" s="5"/>
+      <c r="G50" s="5" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="3" t="s">
+      <c r="I50" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="J50" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6" t="s">
+      <c r="L50" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="I44" s="11" t="s">
+      <c r="Q50" s="30"/>
+      <c r="R50" s="30"/>
+      <c r="S50" s="30"/>
+      <c r="T50" s="30"/>
+      <c r="U50" s="30"/>
+      <c r="V50" s="16"/>
+      <c r="W50" s="10"/>
+      <c r="X50" s="10"/>
+      <c r="AG50" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="J44" s="23" t="s">
+    </row>
+    <row r="51">
+      <c r="A51" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="K44" s="43"/>
-      <c r="L44" s="44" t="s">
+      <c r="B51" s="48" t="s">
         <v>233</v>
       </c>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29" t="s">
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="5"/>
+      <c r="L51" s="28"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="30"/>
+      <c r="S51" s="30"/>
+      <c r="T51" s="30"/>
+      <c r="U51" s="30"/>
+      <c r="V51" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="V44" s="14" t="s">
+      <c r="W51" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="W44" s="11" t="s">
+      <c r="X51" s="10"/>
+      <c r="AG51" s="37"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="X44" s="11"/>
-      <c r="AD44" s="6" t="s">
+      <c r="B52" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AE44" s="6"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="3" t="s">
+      <c r="F52" s="5"/>
+      <c r="G52" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="I52" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="P45" s="9" t="s">
+      <c r="J52" s="24" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="3" t="s">
+      <c r="K52" s="12"/>
+      <c r="L52" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="Q52" s="30"/>
+      <c r="R52" s="30"/>
+      <c r="S52" s="30"/>
+      <c r="T52" s="30"/>
+      <c r="U52" s="30"/>
+      <c r="V52" s="16"/>
+      <c r="W52" s="10"/>
+      <c r="X52" s="10"/>
+      <c r="AD52" s="5"/>
+      <c r="AE52" s="5"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="P46" s="9" t="s">
+      <c r="B53" s="48" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="3" t="s">
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="14"/>
+      <c r="Q53" s="30"/>
+      <c r="R53" s="30"/>
+      <c r="S53" s="30"/>
+      <c r="T53" s="30"/>
+      <c r="U53" s="30"/>
+      <c r="V53" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="W53" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="P47" s="9" t="s">
+      <c r="X53" s="10"/>
+      <c r="AD53" s="5"/>
+      <c r="AE53" s="5"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="3" t="s">
+      <c r="B54" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="P54" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="H48" s="7" t="s">
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="B55" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="O48" s="18" t="s">
+      <c r="P55" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="P48" s="9" t="s">
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1" t="s">
+      <c r="B56" s="47" t="s">
         <v>253</v>
       </c>
-      <c r="V48" s="14" t="s">
+      <c r="P56" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="W48" s="11" t="s">
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="X48" s="11"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="3" t="s">
+      <c r="B57" s="47" t="s">
         <v>256</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="H57" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="P49" s="9" t="s">
+      <c r="I57" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="Q49" s="46" t="s">
+      <c r="O57" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="R49" s="46"/>
-      <c r="S49" s="46"/>
-      <c r="T49" s="46"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="3" t="s">
+      <c r="P57" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="16"/>
+      <c r="W57" s="10"/>
+      <c r="X57" s="10"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="M50" s="17"/>
-      <c r="N50" s="17" t="s">
+      <c r="B58" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="O50" s="47" t="s">
+      <c r="H58" s="6"/>
+      <c r="I58" s="7"/>
+      <c r="O58" s="19"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="P50" s="9" t="s">
+      <c r="W58" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="AD50" s="48"/>
-      <c r="AE50" s="48"/>
-      <c r="AF50" s="48" t="s">
+      <c r="X58" s="10"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="3" t="s">
+      <c r="B59" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="P59" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="P51" s="9" t="s">
+      <c r="Q59" s="48" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="3" t="s">
+      <c r="R59" s="48"/>
+      <c r="S59" s="48"/>
+      <c r="T59" s="48"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B60" s="47" t="s">
         <v>270</v>
       </c>
-      <c r="P52" s="9" t="s">
+      <c r="M60" s="18"/>
+      <c r="N60" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="1" t="s">
+      <c r="O60" s="50" t="s">
         <v>272</v>
       </c>
-      <c r="S52" s="1"/>
-      <c r="U52" s="1" t="s">
+      <c r="P60" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="X52" s="48" t="s">
+      <c r="AD60" s="51"/>
+      <c r="AE60" s="51"/>
+      <c r="AF60" s="51" t="s">
         <v>274</v>
       </c>
-      <c r="Y52" s="29" t="s">
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="AF52" s="49" t="s">
+      <c r="B61" s="47" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="3" t="s">
+      <c r="P61" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="B53" s="42" t="s">
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="P53" s="1" t="s">
+      <c r="B62" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="2" t="s">
+      <c r="P62" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1"/>
-      <c r="U53" s="1" t="s">
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="V53" s="14" t="s">
+      <c r="S62" s="1"/>
+      <c r="X62" s="51"/>
+      <c r="Y62" s="30"/>
+      <c r="AF62" s="52"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="43" t="s">
         <v>282</v>
       </c>
-      <c r="W53" s="1" t="s">
+      <c r="B63" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="X53" s="1"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="3" t="s">
+      <c r="P63" s="8"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="X63" s="51"/>
+      <c r="Y63" s="30"/>
+      <c r="AF63" s="52"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B64" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="P54" s="9" t="s">
+      <c r="P64" s="8"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="X64" s="51"/>
+      <c r="Y64" s="30"/>
+      <c r="AF64" s="52"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="AC54" s="50" t="s">
+      <c r="B65" s="38" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="3" t="s">
+      <c r="P65" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6" t="s">
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="16"/>
+      <c r="X65" s="1"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="I55" s="51" t="s">
+      <c r="B66" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="J55" s="52" t="s">
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="L55" s="53" t="s">
+      <c r="W66" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="P55" s="9" t="s">
+      <c r="X66" s="1"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="Q55" s="2"/>
-      <c r="R55" s="1" t="s">
+      <c r="B67" s="47" t="s">
         <v>295</v>
       </c>
-      <c r="S55" s="1"/>
-      <c r="AD55" s="6" t="s">
+      <c r="P67" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="AE55" s="37" t="s">
+      <c r="AC67" s="53" t="s">
         <v>297</v>
       </c>
-      <c r="AG55" s="54" t="s">
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="3" t="s">
+      <c r="B68" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="F68" s="5"/>
+      <c r="G68" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="P56" s="9" t="s">
+      <c r="I68" s="54" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="3" t="s">
+      <c r="J68" s="55" t="s">
         <v>302</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="L68" s="56" t="s">
         <v>303</v>
       </c>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6" t="s">
+      <c r="P68" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="I57" s="51" t="s">
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="O57" s="47" t="s">
+      <c r="S68" s="1"/>
+      <c r="AD68" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="P57" s="9"/>
-      <c r="AG57" s="54" t="s">
+      <c r="AE68" s="41" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="3" t="s">
+      <c r="AG68" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="B58" s="42" t="s">
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="B69" s="47" t="s">
+        <v>310</v>
+      </c>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="P69" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B70" s="47" t="s">
+        <v>313</v>
+      </c>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="I70" s="54" t="s">
+        <v>315</v>
+      </c>
+      <c r="O70" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="P70" s="8"/>
+      <c r="AG70" s="57" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B71" s="47" t="s">
+        <v>319</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P58" s="9" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="B59" s="42" t="s">
-        <v>312</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="I59" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="L59" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="P59" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
-      <c r="T59" s="1"/>
-      <c r="U59" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="V59" s="55" t="s">
-        <v>319</v>
-      </c>
-      <c r="W59" s="11" t="s">
+      <c r="P71" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="X59" s="11"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="3" t="s">
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B60" s="34" t="s">
+      <c r="B72" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="P60" s="9" t="s">
+      <c r="H72" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="V60" s="56"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="3" t="s">
+      <c r="I72" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="B61" s="42" t="s">
+      <c r="J72" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="P61" s="9" t="s">
+      <c r="L72" s="7" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="3" t="s">
+      <c r="P72" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="B62" s="42" t="s">
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="58"/>
+      <c r="W72" s="10"/>
+      <c r="X72" s="10"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="43" t="s">
+        <v>321</v>
+      </c>
+      <c r="B73" s="48" t="s">
+        <v>322</v>
+      </c>
+      <c r="H73" s="6"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="5"/>
+      <c r="L73" s="7"/>
+      <c r="P73" s="8"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6" t="s">
+      <c r="W73" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="I62" s="51" t="s">
+      <c r="X73" s="10"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="J62" s="52" t="s">
+      <c r="B74" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="L62" s="53" t="s">
+      <c r="P74" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="P62" s="9" t="s">
+      <c r="V74" s="59"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="2" t="s">
+      <c r="B75" s="47" t="s">
         <v>334</v>
       </c>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-      <c r="U62" s="1" t="s">
+      <c r="P75" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="V62" s="55" t="s">
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="W62" s="11" t="s">
+      <c r="B76" s="47" t="s">
         <v>337</v>
       </c>
-      <c r="X62" s="11"/>
-      <c r="AC62" s="21" t="s">
+      <c r="F76" s="5"/>
+      <c r="G76" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="AG62" s="54" t="s">
+      <c r="I76" s="54" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="3" t="s">
+      <c r="J76" s="55" t="s">
         <v>340</v>
       </c>
-      <c r="B63" s="42" t="s">
+      <c r="L76" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="P63" s="9" t="s">
+      <c r="P76" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="R63" s="3"/>
-      <c r="S63" s="3"/>
-      <c r="T63" s="3" t="s">
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="AC63" s="57" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="3" t="s">
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+      <c r="V76" s="58"/>
+      <c r="W76" s="10"/>
+      <c r="X76" s="10"/>
+      <c r="AC76" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="B64" s="42" t="s">
+      <c r="AG76" s="57" t="s">
         <v>345</v>
       </c>
-      <c r="N64" s="17" t="s">
+    </row>
+    <row r="77">
+      <c r="A77" s="43" t="s">
         <v>346</v>
       </c>
-      <c r="P64" s="58"/>
-      <c r="U64" s="29" t="s">
+      <c r="B77" s="48" t="s">
         <v>347</v>
       </c>
-      <c r="X64" s="49" t="s">
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="I77" s="54"/>
+      <c r="J77" s="55"/>
+      <c r="L77" s="56"/>
+      <c r="P77" s="8"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+      <c r="V77" s="58" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="3" t="s">
+      <c r="W77" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="B65" s="42" t="s">
+      <c r="X77" s="10"/>
+      <c r="AC77" s="22"/>
+      <c r="AG77" s="57"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="P65" s="9" t="s">
+      <c r="B78" s="47" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="3" t="s">
+      <c r="P78" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="R78" s="2"/>
+      <c r="S78" s="2"/>
+      <c r="T78" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="P66" s="9" t="s">
+      <c r="AC78" s="60" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="3" t="s">
+      <c r="B79" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="N79" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="P79" s="61"/>
+      <c r="U79" s="30"/>
+      <c r="X79" s="52"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="B80" s="48" t="s">
+        <v>358</v>
+      </c>
+      <c r="N80" s="18"/>
+      <c r="P80" s="61"/>
+      <c r="U80" s="30"/>
+      <c r="X80" s="52" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B81" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="P81" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B82" s="47" t="s">
+        <v>364</v>
+      </c>
+      <c r="P82" s="8" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B83" s="47" t="s">
+        <v>367</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="B68" s="42" t="s">
-        <v>358</v>
-      </c>
-      <c r="P68" s="9" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="B69" s="42" t="s">
-        <v>361</v>
-      </c>
-      <c r="P69" s="9" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="B70" s="42" t="s">
-        <v>364</v>
-      </c>
-      <c r="C70" s="5" t="s">
+    <row r="84">
+      <c r="A84" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B84" s="47" t="s">
+        <v>369</v>
+      </c>
+      <c r="P84" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B85" s="47" t="s">
+        <v>372</v>
+      </c>
+      <c r="P85" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B86" s="47" t="s">
+        <v>375</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="C71" s="5" t="s">
+    <row r="87">
+      <c r="A87" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B72" s="42" t="s">
-        <v>368</v>
-      </c>
-      <c r="P72" s="9" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="B73" s="42" t="s">
-        <v>371</v>
-      </c>
-      <c r="C73" s="5" t="s">
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B88" s="47" t="s">
+        <v>379</v>
+      </c>
+      <c r="P88" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B89" s="47" t="s">
+        <v>382</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="B74" s="42" t="s">
-        <v>373</v>
-      </c>
-      <c r="C74" s="5" t="s">
+    <row r="90">
+      <c r="A90" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B90" s="47" t="s">
+        <v>384</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P74" s="59" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B75" s="42" t="s">
-        <v>376</v>
-      </c>
-      <c r="P75" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="R75" s="29" t="s">
-        <v>378</v>
-      </c>
-      <c r="S75" s="29"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="B76" s="42" t="s">
-        <v>380</v>
-      </c>
-      <c r="P76" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="R76" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="S76" s="1"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="B77" s="42" t="s">
-        <v>384</v>
-      </c>
-      <c r="P77" s="9" t="s">
+      <c r="P90" s="62" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="3" t="s">
+    <row r="91">
+      <c r="A91" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B78" s="42" t="s">
+      <c r="B91" s="47" t="s">
         <v>387</v>
       </c>
-      <c r="P78" s="9" t="s">
+      <c r="P91" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="AC78" s="60" t="s">
+      <c r="R91" s="30" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="3" t="s">
+      <c r="S91" s="30"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B79" s="42" t="s">
+      <c r="B92" s="47" t="s">
         <v>391</v>
       </c>
-      <c r="D79" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="P79" s="9" t="s">
+      <c r="P92" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="R79" s="1" t="s">
+      <c r="R92" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="S79" s="1"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="3" t="s">
+      <c r="S92" s="1"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B80" s="42" t="s">
+      <c r="B93" s="47" t="s">
         <v>395</v>
       </c>
-      <c r="P80" s="9" t="s">
+      <c r="P93" s="8" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="3" t="s">
+    <row r="94">
+      <c r="A94" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="B94" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="P94" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="AC94" s="63" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B95" s="47" t="s">
+        <v>402</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="P95" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="R95" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="S95" s="1"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B96" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="P96" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B97" s="47" t="s">
+        <v>409</v>
+      </c>
+      <c r="C97" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P81" s="9" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="B82" s="42" t="s">
-        <v>401</v>
-      </c>
-      <c r="P82" s="9" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="B83" s="42" t="s">
-        <v>404</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="B84" s="42" t="s">
-        <v>406</v>
-      </c>
-      <c r="P84" s="9" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="B85" s="42" t="s">
-        <v>409</v>
-      </c>
-      <c r="H85" s="7" t="s">
+      <c r="P97" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="I85" s="51" t="s">
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="O85" s="47" t="s">
+      <c r="B98" s="47" t="s">
         <v>412</v>
       </c>
-      <c r="P85" s="9" t="s">
+      <c r="P98" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="Q85" s="29"/>
-      <c r="R85" s="29" t="s">
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="S85" s="29"/>
-      <c r="T85" s="29"/>
-      <c r="U85" s="29" t="s">
+      <c r="B99" s="47" t="s">
         <v>415</v>
       </c>
-      <c r="V85" s="55" t="s">
+      <c r="D99" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="W85" s="37" t="s">
+      <c r="B100" s="47" t="s">
         <v>417</v>
       </c>
-      <c r="X85" s="37"/>
-      <c r="AB85" s="9" t="s">
+      <c r="P100" s="8" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="3" t="s">
+    <row r="101">
+      <c r="A101" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B86" s="42" t="s">
+      <c r="B101" s="38" t="s">
         <v>420</v>
       </c>
-      <c r="H86" s="17" t="s">
+      <c r="H101" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="I86" s="61" t="s">
+      <c r="I101" s="54" t="s">
         <v>422</v>
       </c>
-      <c r="M86" s="61"/>
-      <c r="N86" s="61" t="s">
+      <c r="O101" s="50" t="s">
         <v>423</v>
       </c>
-      <c r="P86" s="9" t="s">
+      <c r="P101" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="Q86" s="29"/>
-      <c r="R86" s="29"/>
-      <c r="S86" s="29"/>
-      <c r="T86" s="29"/>
-      <c r="U86" s="29" t="s">
+      <c r="Q101" s="30"/>
+      <c r="R101" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="V86" s="55" t="s">
+      <c r="S101" s="30"/>
+      <c r="T101" s="30"/>
+      <c r="U101" s="30"/>
+      <c r="V101" s="58"/>
+      <c r="W101" s="41"/>
+      <c r="X101" s="41"/>
+      <c r="AB101" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="W86" s="37" t="s">
+    </row>
+    <row r="102">
+      <c r="A102" s="43" t="s">
         <v>427</v>
       </c>
-      <c r="X86" s="37"/>
-      <c r="AG86" s="54" t="s">
+      <c r="B102" s="48" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="3" t="s">
+      <c r="H102" s="6"/>
+      <c r="I102" s="54"/>
+      <c r="O102" s="50"/>
+      <c r="P102" s="8"/>
+      <c r="Q102" s="30"/>
+      <c r="R102" s="30"/>
+      <c r="S102" s="30"/>
+      <c r="T102" s="30"/>
+      <c r="U102" s="30"/>
+      <c r="V102" s="58" t="s">
         <v>429</v>
       </c>
-      <c r="B87" s="42" t="s">
+      <c r="W102" s="41" t="s">
         <v>430</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="X102" s="41"/>
+      <c r="AB102" s="8"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B103" s="47" t="s">
+        <v>432</v>
+      </c>
+      <c r="H103" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="I103" s="64" t="s">
+        <v>434</v>
+      </c>
+      <c r="M103" s="64"/>
+      <c r="N103" s="64" t="s">
+        <v>435</v>
+      </c>
+      <c r="P103" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q103" s="30"/>
+      <c r="R103" s="30"/>
+      <c r="S103" s="30"/>
+      <c r="T103" s="30"/>
+      <c r="U103" s="30"/>
+      <c r="V103" s="58"/>
+      <c r="W103" s="41"/>
+      <c r="X103" s="41"/>
+      <c r="AG103" s="57" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="43" t="s">
+        <v>438</v>
+      </c>
+      <c r="B104" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="H104" s="18"/>
+      <c r="I104" s="64"/>
+      <c r="M104" s="64"/>
+      <c r="N104" s="64"/>
+      <c r="P104" s="8"/>
+      <c r="Q104" s="30"/>
+      <c r="R104" s="30"/>
+      <c r="S104" s="30"/>
+      <c r="T104" s="30"/>
+      <c r="U104" s="30"/>
+      <c r="V104" s="58" t="s">
+        <v>440</v>
+      </c>
+      <c r="W104" s="41" t="s">
+        <v>441</v>
+      </c>
+      <c r="X104" s="41"/>
+      <c r="AG104" s="57"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B105" s="47" t="s">
+        <v>443</v>
+      </c>
+      <c r="E105" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="B88" s="42" t="s">
-        <v>432</v>
-      </c>
-      <c r="M88" s="18" t="s">
-        <v>433</v>
-      </c>
-      <c r="N88" s="17" t="s">
-        <v>434</v>
-      </c>
-      <c r="O88" s="62"/>
-      <c r="P88" s="9" t="s">
-        <v>435</v>
-      </c>
-      <c r="AG88" s="18" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="B89" s="42" t="s">
-        <v>438</v>
-      </c>
-      <c r="P89" s="63"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="B90" s="42" t="s">
-        <v>440</v>
-      </c>
-      <c r="P90" s="64" t="s">
-        <v>441</v>
-      </c>
-      <c r="Q90" s="63" t="s">
-        <v>442</v>
-      </c>
-      <c r="R90" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="S90" s="1"/>
-      <c r="AC90" s="42"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="3" t="s">
+    <row r="106">
+      <c r="A106" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B91" s="42" t="s">
+      <c r="B106" s="47" t="s">
         <v>445</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="M106" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="N106" s="18" t="s">
+        <v>447</v>
+      </c>
+      <c r="O106" s="65"/>
+      <c r="P106" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="AG106" s="19" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B107" s="47" t="s">
+        <v>451</v>
+      </c>
+      <c r="P107" s="66" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B108" s="47" t="s">
+        <v>454</v>
+      </c>
+      <c r="P108" s="67" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q108" s="68" t="s">
+        <v>456</v>
+      </c>
+      <c r="R108" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="S108" s="1"/>
+      <c r="AC108" s="47"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B109" s="47" t="s">
+        <v>459</v>
+      </c>
+      <c r="C109" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="B92" s="42" t="s">
-        <v>447</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="B93" s="42" t="s">
-        <v>449</v>
-      </c>
-      <c r="J93" s="40" t="s">
-        <v>450</v>
-      </c>
-      <c r="W93" s="37" t="s">
-        <v>451</v>
-      </c>
-      <c r="X93" s="37"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="B94" s="42" t="s">
-        <v>453</v>
-      </c>
-      <c r="F94" s="6"/>
-      <c r="G94" s="6" t="s">
-        <v>454</v>
-      </c>
-      <c r="I94" s="51" t="s">
-        <v>455</v>
-      </c>
-      <c r="J94" s="52" t="s">
-        <v>456</v>
-      </c>
-      <c r="K94" s="53"/>
-      <c r="L94" s="53" t="s">
-        <v>457</v>
-      </c>
-      <c r="P94" s="21" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q94" s="65"/>
-      <c r="R94" s="65"/>
-      <c r="S94" s="65"/>
-      <c r="T94" s="65"/>
-      <c r="U94" s="65" t="s">
-        <v>459</v>
-      </c>
-      <c r="V94" s="55" t="s">
+    <row r="110">
+      <c r="A110" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="W94" s="37" t="s">
+      <c r="B110" s="47" t="s">
         <v>461</v>
       </c>
-      <c r="X94" s="37"/>
-      <c r="AG94" s="38" t="s">
+      <c r="D110" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="3" t="s">
+      <c r="B111" s="47" t="s">
         <v>463</v>
       </c>
-      <c r="B95" s="42" t="s">
+      <c r="J111" s="45" t="s">
         <v>464</v>
       </c>
-      <c r="P95" s="9" t="s">
+      <c r="W111" s="41" t="s">
         <v>465</v>
       </c>
-      <c r="Q95" s="29"/>
-      <c r="R95" s="29"/>
-      <c r="S95" s="29"/>
-      <c r="T95" s="29"/>
-      <c r="U95" s="29" t="s">
+      <c r="X111" s="41"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="V95" s="55" t="s">
+      <c r="B112" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="W95" s="37" t="s">
+      <c r="F112" s="5"/>
+      <c r="G112" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="X95" s="37"/>
-    </row>
-    <row r="96">
-      <c r="A96" s="3" t="s">
+      <c r="I112" s="54" t="s">
         <v>469</v>
       </c>
-      <c r="B96" s="42" t="s">
+      <c r="J112" s="55" t="s">
         <v>470</v>
       </c>
-      <c r="P96" s="9" t="s">
+      <c r="K112" s="56"/>
+      <c r="L112" s="56" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="3" t="s">
+      <c r="P112" s="22" t="s">
         <v>472</v>
       </c>
-      <c r="B97" s="42" t="s">
+      <c r="Q112" s="69"/>
+      <c r="R112" s="69"/>
+      <c r="S112" s="69"/>
+      <c r="T112" s="69"/>
+      <c r="U112" s="69"/>
+      <c r="V112" s="58"/>
+      <c r="W112" s="41"/>
+      <c r="X112" s="41"/>
+      <c r="AG112" s="42" t="s">
         <v>473</v>
       </c>
-      <c r="P97" s="21" t="s">
+    </row>
+    <row r="113">
+      <c r="A113" s="43" t="s">
         <v>474</v>
       </c>
-      <c r="AC97" s="60" t="s">
+      <c r="B113" s="48" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="3" t="s">
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="I113" s="54"/>
+      <c r="J113" s="55"/>
+      <c r="K113" s="56"/>
+      <c r="L113" s="56"/>
+      <c r="P113" s="22"/>
+      <c r="Q113" s="69"/>
+      <c r="R113" s="69"/>
+      <c r="S113" s="69"/>
+      <c r="T113" s="69"/>
+      <c r="U113" s="69"/>
+      <c r="V113" s="58" t="s">
         <v>476</v>
       </c>
-      <c r="B98" s="42" t="s">
+      <c r="W113" s="41" t="s">
         <v>477</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="X113" s="41"/>
+      <c r="AG113" s="42"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B114" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="P114" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q114" s="30"/>
+      <c r="R114" s="30"/>
+      <c r="S114" s="30"/>
+      <c r="T114" s="30"/>
+      <c r="U114" s="30"/>
+      <c r="V114" s="58"/>
+      <c r="W114" s="41"/>
+      <c r="X114" s="41"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="43" t="s">
+        <v>481</v>
+      </c>
+      <c r="B115" s="48" t="s">
+        <v>482</v>
+      </c>
+      <c r="P115" s="8"/>
+      <c r="Q115" s="30"/>
+      <c r="R115" s="30"/>
+      <c r="S115" s="30"/>
+      <c r="T115" s="30"/>
+      <c r="U115" s="30"/>
+      <c r="V115" s="58" t="s">
+        <v>483</v>
+      </c>
+      <c r="W115" s="41" t="s">
+        <v>484</v>
+      </c>
+      <c r="X115" s="41"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B116" s="47" t="s">
+        <v>486</v>
+      </c>
+      <c r="P116" s="8" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B117" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="P117" s="22" t="s">
+        <v>490</v>
+      </c>
+      <c r="AC117" s="63" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B118" s="47" t="s">
+        <v>493</v>
+      </c>
+      <c r="C118" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="B99" s="42" t="s">
-        <v>479</v>
-      </c>
-      <c r="F99" s="17" t="s">
-        <v>480</v>
-      </c>
-      <c r="H99" s="7"/>
-      <c r="K99" s="66" t="s">
-        <v>481</v>
-      </c>
-      <c r="L99" s="8" t="s">
-        <v>482</v>
-      </c>
-      <c r="U99" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="V99" s="55" t="s">
-        <v>484</v>
-      </c>
-      <c r="W99" s="37" t="s">
-        <v>485</v>
-      </c>
-      <c r="X99" s="37"/>
-    </row>
-    <row r="100">
-      <c r="A100" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="B100" s="42" t="s">
-        <v>487</v>
-      </c>
-      <c r="F100" s="17" t="s">
-        <v>488</v>
-      </c>
-      <c r="M100" s="17"/>
-      <c r="N100" s="17"/>
-      <c r="O100" s="47" t="s">
-        <v>489</v>
-      </c>
-      <c r="P100" s="9" t="s">
-        <v>490</v>
-      </c>
-      <c r="Q100" s="29"/>
-      <c r="R100" s="29"/>
-      <c r="S100" s="29"/>
-      <c r="T100" s="29"/>
-      <c r="U100" s="29" t="s">
-        <v>491</v>
-      </c>
-      <c r="V100" s="55" t="s">
-        <v>492</v>
-      </c>
-      <c r="W100" s="37" t="s">
-        <v>493</v>
-      </c>
-      <c r="X100" s="37"/>
-      <c r="AC100" s="3" t="s">
+    <row r="119">
+      <c r="A119" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="AD100" s="6" t="s">
+      <c r="B119" s="47" t="s">
         <v>495</v>
       </c>
-      <c r="AE100" s="8" t="s">
+      <c r="F119" s="18" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="3" t="s">
+      <c r="H119" s="6"/>
+      <c r="K119" s="70" t="s">
         <v>497</v>
       </c>
-      <c r="B101" s="42" t="s">
+      <c r="L119" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="P101" s="9" t="s">
+      <c r="U119" s="71"/>
+      <c r="V119" s="58"/>
+      <c r="W119" s="41"/>
+      <c r="X119" s="41"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="43" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="3" t="s">
+      <c r="B120" s="48" t="s">
         <v>500</v>
       </c>
-      <c r="B102" s="42" t="s">
+      <c r="F120" s="18"/>
+      <c r="H120" s="6"/>
+      <c r="K120" s="70"/>
+      <c r="L120" s="7"/>
+      <c r="U120" s="1"/>
+      <c r="V120" s="58" t="s">
         <v>501</v>
       </c>
-      <c r="P102" s="9" t="s">
+      <c r="W120" s="41" t="s">
         <v>502</v>
       </c>
-      <c r="AG102" s="54" t="s">
+      <c r="X120" s="41"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="3" t="s">
+      <c r="B121" s="47" t="s">
         <v>504</v>
       </c>
-      <c r="B103" s="42" t="s">
+      <c r="F121" s="18" t="s">
         <v>505</v>
       </c>
-      <c r="P103" s="21" t="s">
+      <c r="M121" s="18"/>
+      <c r="N121" s="18"/>
+      <c r="O121" s="50" t="s">
         <v>506</v>
       </c>
-      <c r="AC103" s="21" t="s">
+      <c r="P121" s="8" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="3" t="s">
+      <c r="Q121" s="30"/>
+      <c r="R121" s="30"/>
+      <c r="S121" s="30"/>
+      <c r="T121" s="30"/>
+      <c r="U121" s="30"/>
+      <c r="V121" s="58"/>
+      <c r="W121" s="41"/>
+      <c r="X121" s="41"/>
+      <c r="AC121" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="B104" s="42" t="s">
+      <c r="AD121" s="5"/>
+      <c r="AE121" s="7"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="33" t="s">
         <v>509</v>
       </c>
-      <c r="D104" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H104" s="7" t="s">
+      <c r="B122" s="48" t="s">
         <v>510</v>
       </c>
-      <c r="I104" s="11" t="s">
+      <c r="F122" s="18"/>
+      <c r="M122" s="18"/>
+      <c r="N122" s="18"/>
+      <c r="O122" s="50"/>
+      <c r="P122" s="8"/>
+      <c r="Q122" s="30"/>
+      <c r="R122" s="30"/>
+      <c r="S122" s="30"/>
+      <c r="T122" s="30"/>
+      <c r="U122" s="30"/>
+      <c r="V122" s="58" t="s">
         <v>511</v>
       </c>
-      <c r="J104" s="23" t="s">
+      <c r="W122" s="41" t="s">
         <v>512</v>
       </c>
-      <c r="L104" s="44" t="s">
+      <c r="X122" s="41"/>
+      <c r="AC122" s="2"/>
+      <c r="AD122" s="5"/>
+      <c r="AE122" s="7"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="3" t="s">
+      <c r="B123" s="38" t="s">
         <v>514</v>
       </c>
-      <c r="B105" s="42" t="s">
+      <c r="P123" s="8" t="s">
         <v>515</v>
       </c>
-      <c r="P105" s="9" t="s">
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="R105" s="1" t="s">
+      <c r="B124" s="47" t="s">
         <v>517</v>
       </c>
-      <c r="S105" s="2" t="s">
+      <c r="P124" s="8" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="3" t="s">
+      <c r="AG124" s="57" t="s">
         <v>519</v>
       </c>
-      <c r="B106" s="3" t="s">
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="P106" s="9" t="s">
+      <c r="B125" s="47" t="s">
         <v>521</v>
       </c>
-      <c r="Q106" s="29"/>
-      <c r="R106" s="29"/>
-      <c r="S106" s="29"/>
-      <c r="T106" s="29"/>
-      <c r="U106" s="29" t="s">
+      <c r="P125" s="22" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="3" t="s">
+      <c r="AC125" s="22" t="s">
         <v>523</v>
       </c>
-      <c r="B107" s="42" t="s">
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="B126" s="47" t="s">
+        <v>525</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H126" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="I126" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="J126" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="L126" s="14" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B127" s="38" t="s">
+        <v>531</v>
+      </c>
+      <c r="P127" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="R127" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="S127" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="P128" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q128" s="30"/>
+      <c r="R128" s="30"/>
+      <c r="S128" s="30"/>
+      <c r="T128" s="30"/>
+      <c r="U128" s="30"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="43" t="s">
+        <v>538</v>
+      </c>
+      <c r="B129" s="43" t="s">
+        <v>539</v>
+      </c>
+      <c r="P129" s="8"/>
+      <c r="Q129" s="30"/>
+      <c r="R129" s="30"/>
+      <c r="S129" s="30"/>
+      <c r="T129" s="30"/>
+      <c r="U129" s="30"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B130" s="47" t="s">
+        <v>541</v>
+      </c>
+      <c r="C130" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P107" s="9" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="B108" s="42" t="s">
-        <v>527</v>
-      </c>
-      <c r="H108" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="I108" s="51" t="s">
-        <v>529</v>
-      </c>
-      <c r="O108" s="67" t="s">
-        <v>530</v>
-      </c>
-      <c r="P108" s="9" t="s">
-        <v>531</v>
-      </c>
-      <c r="Q108" s="29"/>
-      <c r="R108" s="29"/>
-      <c r="S108" s="29"/>
-      <c r="T108" s="29"/>
-      <c r="U108" s="29" t="s">
-        <v>532</v>
-      </c>
-      <c r="V108" s="55" t="s">
-        <v>533</v>
-      </c>
-      <c r="W108" s="37" t="s">
-        <v>534</v>
-      </c>
-      <c r="X108" s="37"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="B109" s="42" t="s">
-        <v>536</v>
-      </c>
-      <c r="C109" s="5" t="s">
+      <c r="P130" s="8" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="B131" s="47" t="s">
+        <v>544</v>
+      </c>
+      <c r="H131" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="I131" s="54" t="s">
+        <v>546</v>
+      </c>
+      <c r="O131" s="72" t="s">
+        <v>547</v>
+      </c>
+      <c r="P131" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q131" s="30"/>
+      <c r="R131" s="30"/>
+      <c r="S131" s="30"/>
+      <c r="T131" s="30"/>
+      <c r="U131" s="30"/>
+      <c r="V131" s="58"/>
+      <c r="W131" s="41"/>
+      <c r="X131" s="41"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="33" t="s">
+        <v>549</v>
+      </c>
+      <c r="B132" s="48" t="s">
+        <v>550</v>
+      </c>
+      <c r="H132" s="6"/>
+      <c r="I132" s="54"/>
+      <c r="O132" s="72"/>
+      <c r="P132" s="8"/>
+      <c r="Q132" s="30"/>
+      <c r="R132" s="30"/>
+      <c r="S132" s="30"/>
+      <c r="T132" s="30"/>
+      <c r="U132" s="30"/>
+      <c r="V132" s="58" t="s">
+        <v>551</v>
+      </c>
+      <c r="W132" s="41" t="s">
+        <v>552</v>
+      </c>
+      <c r="X132" s="41"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B133" s="47" t="s">
+        <v>554</v>
+      </c>
+      <c r="C133" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="B110" s="42" t="s">
-        <v>538</v>
-      </c>
-      <c r="C110" s="5" t="s">
+    <row r="134">
+      <c r="A134" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B134" s="47" t="s">
+        <v>556</v>
+      </c>
+      <c r="C134" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="B111" s="42" t="s">
-        <v>540</v>
-      </c>
-      <c r="P111" s="9" t="s">
-        <v>541</v>
+    <row r="135">
+      <c r="A135" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B135" s="47" t="s">
+        <v>558</v>
+      </c>
+      <c r="P135" s="8" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>